<commit_message>
add links to table
</commit_message>
<xml_diff>
--- a/excel_test.xlsx
+++ b/excel_test.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t xml:space="preserve">Anna, Müller</t>
   </si>
@@ -211,10 +211,10 @@
     <t xml:space="preserve">League 5</t>
   </si>
   <si>
-    <t xml:space="preserve">League 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">League 7</t>
+    <t xml:space="preserve">https://lichess.org/@/Bastiu16293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lichess.org/@/delta2206</t>
   </si>
 </sst>
 </file>
@@ -229,6 +229,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -249,12 +250,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -305,16 +308,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -799,275 +810,339 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:H16"/>
+  <dimension ref="B3:M13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="31.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="28.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="27.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="25.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="2" width="19.33"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="str">
+      <c r="B4" s="2" t="str">
         <f aca="false">Players!$B2</f>
         <v>Anna, Müller</v>
       </c>
-      <c r="C4" s="0" t="str">
+      <c r="C4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="2" t="str">
         <f aca="false">Players!$B10</f>
         <v>Maria, Braun</v>
       </c>
-      <c r="D4" s="0" t="str">
+      <c r="E4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="2" t="str">
         <f aca="false">Players!$B16</f>
         <v>Emma, Hartmann</v>
       </c>
-      <c r="E4" s="0" t="str">
+      <c r="G4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="2" t="str">
         <f aca="false">Players!$B26</f>
         <v>Katharina, Schreiber</v>
       </c>
-      <c r="F4" s="0" t="str">
+      <c r="I4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="2" t="str">
         <f aca="false">Players!$B33</f>
         <v>Adrian, Lange</v>
       </c>
-      <c r="G4" s="0" t="str">
-        <f aca="false">Players!$B38</f>
-        <v>Jonathan, Lange</v>
-      </c>
-      <c r="H4" s="0" t="str">
-        <f aca="false">Players!$B40</f>
-        <v>Tobias, Winkler</v>
+      <c r="K4" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="str">
+      <c r="B5" s="2" t="str">
         <f aca="false">Players!$B3</f>
         <v>Max, Schmidt</v>
       </c>
-      <c r="C5" s="0" t="str">
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="2" t="str">
         <f aca="false">Players!$B11</f>
         <v>Markus, Fischer</v>
       </c>
-      <c r="D5" s="0" t="str">
+      <c r="E5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="2" t="str">
         <f aca="false">Players!$B17</f>
         <v>Paul, Koch</v>
       </c>
-      <c r="E5" s="0" t="str">
+      <c r="G5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="2" t="str">
         <f aca="false">Players!$B27</f>
         <v>Christian, Weber</v>
       </c>
-      <c r="F5" s="0" t="str">
+      <c r="I5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="2" t="str">
         <f aca="false">Players!$B34</f>
         <v>Nicole, Meyer</v>
       </c>
-      <c r="G5" s="0" t="str">
-        <f aca="false">Players!$B39</f>
-        <v>Eva, Koch</v>
-      </c>
-      <c r="H5" s="0" t="str">
-        <f aca="false">Players!$B41</f>
-        <v>Nina, Petersen</v>
+      <c r="K5" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="str">
+      <c r="B6" s="2" t="str">
         <f aca="false">Players!$B4</f>
         <v>Julia, Becker</v>
       </c>
-      <c r="C6" s="0" t="str">
+      <c r="C6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="2" t="str">
         <f aca="false">Players!$B12</f>
         <v>Lena, Meyer</v>
       </c>
-      <c r="D6" s="0" t="str">
+      <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="2" t="str">
         <f aca="false">Players!$B18</f>
         <v>Clara, Schmidt</v>
       </c>
-      <c r="E6" s="0" t="str">
+      <c r="G6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="2" t="str">
         <f aca="false">Players!$B28</f>
         <v>Melanie, Horn</v>
       </c>
-      <c r="F6" s="0" t="str">
+      <c r="I6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="2" t="str">
         <f aca="false">Players!$B35</f>
         <v>Janis, Schneider</v>
       </c>
-      <c r="H6" s="0" t="str">
-        <f aca="false">Players!$B42</f>
-        <v>Alexander, Schulze</v>
+      <c r="K6" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="str">
+      <c r="B7" s="2" t="str">
         <f aca="false">Players!$B5</f>
         <v>Tom, Wagner</v>
       </c>
-      <c r="C7" s="0" t="str">
+      <c r="C7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="2" t="str">
         <f aca="false">Players!$B13</f>
         <v>Michael, Richter</v>
       </c>
-      <c r="D7" s="0" t="str">
+      <c r="E7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="2" t="str">
         <f aca="false">Players!$B19</f>
         <v>Tim, Braun</v>
       </c>
-      <c r="E7" s="0" t="str">
+      <c r="G7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="2" t="str">
         <f aca="false">Players!$B29</f>
         <v>Johannes, Neumann</v>
       </c>
-      <c r="F7" s="0" t="str">
+      <c r="I7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="2" t="str">
         <f aca="false">Players!$B36</f>
         <v>Benjamin, Krämer</v>
       </c>
-      <c r="H7" s="0" t="str">
-        <f aca="false">Players!$B43</f>
-        <v>Julia, Stark</v>
+      <c r="K7" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="str">
+      <c r="B8" s="2" t="str">
         <f aca="false">Players!$B6</f>
         <v>Laura, Klein</v>
       </c>
-      <c r="C8" s="0" t="str">
+      <c r="C8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="2" t="str">
         <f aca="false">Players!$B14</f>
         <v>Sophie, Schäfer</v>
       </c>
-      <c r="D8" s="0" t="str">
+      <c r="E8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2" t="str">
         <f aca="false">Players!$B20</f>
         <v>Isabel, Maier</v>
       </c>
-      <c r="E8" s="0" t="str">
+      <c r="G8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="2" t="str">
         <f aca="false">Players!$B30</f>
         <v>Miriam, Braun</v>
       </c>
-      <c r="F8" s="0" t="str">
+      <c r="I8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="2" t="str">
         <f aca="false">Players!$B37</f>
         <v>Sarah, Vogel</v>
       </c>
-      <c r="H8" s="0" t="str">
-        <f aca="false">Players!$B44</f>
-        <v>Fabian, Huber</v>
+      <c r="K8" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="str">
+      <c r="B9" s="2" t="str">
         <f aca="false">Players!$B7</f>
         <v>Lukas, Hoffmann</v>
       </c>
-      <c r="C9" s="0" t="str">
+      <c r="C9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2" t="str">
         <f aca="false">Players!$B15</f>
         <v>Daniel, Zimmermann</v>
       </c>
-      <c r="D9" s="0" t="str">
+      <c r="E9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="2" t="str">
         <f aca="false">Players!$B21</f>
         <v>Florian, Schmitt</v>
       </c>
-      <c r="E9" s="0" t="str">
+      <c r="G9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="2" t="str">
         <f aca="false">Players!$B31</f>
         <v>Oliver, Fröhlich</v>
       </c>
-      <c r="H9" s="0" t="str">
-        <f aca="false">Players!$B45</f>
-        <v>Johanna, Kühn</v>
+      <c r="I9" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="str">
+      <c r="B10" s="2" t="str">
         <f aca="false">Players!$B8</f>
         <v>Sarah, Weber</v>
       </c>
-      <c r="C10" s="0" t="str">
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="2" t="str">
         <f aca="false">Players!$B16</f>
         <v>Emma, Hartmann</v>
       </c>
-      <c r="D10" s="0" t="str">
+      <c r="E10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="2" t="str">
         <f aca="false">Players!$B22</f>
         <v>Nadine, Keller</v>
       </c>
-      <c r="E10" s="0" t="str">
+      <c r="G10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="2" t="str">
         <f aca="false">Players!$B32</f>
         <v>Jasmin, Roth</v>
       </c>
-      <c r="H10" s="0" t="str">
-        <f aca="false">Players!$B46</f>
-        <v>Thomas, Berger</v>
+      <c r="I10" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="str">
+      <c r="B11" s="2" t="str">
         <f aca="false">Players!$B9</f>
         <v>Peter, Schulz</v>
       </c>
-      <c r="D11" s="0" t="str">
+      <c r="C11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="2" t="str">
         <f aca="false">Players!$B23</f>
         <v>David, Wolf</v>
       </c>
-      <c r="H11" s="0" t="str">
-        <f aca="false">Players!$B47</f>
-        <v>Lisa, Fuchs</v>
+      <c r="G11" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="0" t="str">
+      <c r="F12" s="2" t="str">
         <f aca="false">Players!$B24</f>
         <v>Tanja, Lange</v>
       </c>
-      <c r="H12" s="0" t="str">
-        <f aca="false">Players!$B48</f>
-        <v>Gregor, Hartmann</v>
+      <c r="G12" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="0" t="str">
+      <c r="F13" s="2" t="str">
         <f aca="false">Players!$B25</f>
         <v>Simon, Schwarz</v>
       </c>
-      <c r="H13" s="0" t="str">
-        <f aca="false">Players!$B49</f>
-        <v>Leonie, Müller</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H14" s="0" t="str">
-        <f aca="false">Players!$B50</f>
-        <v>Nico, Weiß</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="0" t="str">
-        <f aca="false">Players!$B51</f>
-        <v>Marlene, Hofmann</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H16" s="0" t="str">
-        <f aca="false">Players!$B52</f>
-        <v>Philipp, Richter</v>
+      <c r="G13" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>